<commit_message>
Appended source files + minor changes
* Cleaned up issue with numeric raw subject grade variables in YCS10 and YCS11. These were string variables for all other YCS cohorts. Used decode command in '2_ycs10_gsce_subjects' & '2_ycs11_gsce_subjects'.

* Corrected mistaken omission of t0examst, t0examac, t0examaf and t0score from YCS5, YCS7, YCS8 & YCS9.

* Ordered variables and created two datasets:
	* 'ycs5_to_11_set1.dta' contains all variables
	* 'ycs5_to_11_set2.dta' is a subset of variables

* If we change our mind, we can return to this.

* Contemplating that I might want to record the highest score (not just highest A*-C) in 18 main subjects.
</commit_message>
<xml_diff>
--- a/ycs_gcse_subjects_variables.xlsx
+++ b/ycs_gcse_subjects_variables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12114" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5049" uniqueCount="452">
   <si>
     <t>variable number</t>
   </si>
@@ -1194,64 +1194,22 @@
     <t>Studied Other GCSE subject 9</t>
   </si>
   <si>
+    <t>ycs10_id</t>
+  </si>
+  <si>
     <t>double</t>
   </si>
   <si>
-    <t>%10.0g</t>
-  </si>
-  <si>
-    <t>a11_1c</t>
-  </si>
-  <si>
-    <t>a11_2c</t>
-  </si>
-  <si>
-    <t>a11_3c</t>
-  </si>
-  <si>
-    <t>a11_6c</t>
-  </si>
-  <si>
-    <t>a11_5c</t>
-  </si>
-  <si>
-    <t>a11_4c</t>
-  </si>
-  <si>
-    <t>a11_8c</t>
-  </si>
-  <si>
-    <t>a11_11c</t>
-  </si>
-  <si>
-    <t>a11_11d</t>
-  </si>
-  <si>
-    <t>a11ogc1</t>
-  </si>
-  <si>
-    <t>a11ogc2</t>
-  </si>
-  <si>
-    <t>a11ogc3</t>
-  </si>
-  <si>
-    <t>a11_9c</t>
-  </si>
-  <si>
-    <t>a11ogc4</t>
-  </si>
-  <si>
-    <t>a11ogc5</t>
-  </si>
-  <si>
-    <t>a11_7c</t>
-  </si>
-  <si>
-    <t>a11ogc6</t>
-  </si>
-  <si>
-    <t>a11_10c</t>
+    <t>str4</t>
+  </si>
+  <si>
+    <t>%9s</t>
+  </si>
+  <si>
+    <t>id for time series</t>
+  </si>
+  <si>
+    <t>ID variable created - based on position in YCS10</t>
   </si>
   <si>
     <t>a11_1c  what result did you get in your english language gcse exam in years 10 a</t>
@@ -1344,69 +1302,15 @@
     <t>t0gcst15a</t>
   </si>
   <si>
-    <t>%23.0g</t>
+    <t>str19</t>
+  </si>
+  <si>
+    <t>%19s</t>
   </si>
   <si>
     <t>sn</t>
   </si>
   <si>
-    <t>s1q15a2</t>
-  </si>
-  <si>
-    <t>s1q15b2</t>
-  </si>
-  <si>
-    <t>s1q15c2</t>
-  </si>
-  <si>
-    <t>s1q15i2</t>
-  </si>
-  <si>
-    <t>s1q15h2</t>
-  </si>
-  <si>
-    <t>s1q15f2</t>
-  </si>
-  <si>
-    <t>s1q15e2</t>
-  </si>
-  <si>
-    <t>s1q15d2</t>
-  </si>
-  <si>
-    <t>s1q15n3</t>
-  </si>
-  <si>
-    <t>s1q15l2</t>
-  </si>
-  <si>
-    <t>s1q15o3</t>
-  </si>
-  <si>
-    <t>s1q15p3</t>
-  </si>
-  <si>
-    <t>s1q15g2</t>
-  </si>
-  <si>
-    <t>s1q15q3</t>
-  </si>
-  <si>
-    <t>s1q15k2</t>
-  </si>
-  <si>
-    <t>s1q15r3</t>
-  </si>
-  <si>
-    <t>s1q15j2</t>
-  </si>
-  <si>
-    <t>s1q15s3</t>
-  </si>
-  <si>
-    <t>s1q15m2</t>
-  </si>
-  <si>
     <t>GCSE Other Science A-C</t>
   </si>
   <si>
@@ -1471,15 +1375,6 @@
   </si>
   <si>
     <t>Studied GCSE RE</t>
-  </si>
-  <si>
-    <t>ycs10_id</t>
-  </si>
-  <si>
-    <t>id for time series</t>
-  </si>
-  <si>
-    <t>ID variable created - based on position in YCS10</t>
   </si>
 </sst>
 </file>
@@ -18306,7 +18201,7 @@
         <v>148</v>
       </c>
       <c r="G3" t="s">
-        <v>485</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4">
@@ -18314,7 +18209,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>484</v>
+        <v>391</v>
       </c>
       <c r="C4" t="s">
         <v>135</v>
@@ -18329,7 +18224,7 @@
         <v>148</v>
       </c>
       <c r="G4" t="s">
-        <v>486</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5">
@@ -18915,7 +18810,7 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D30" s="0">
         <v>1</v>
@@ -18984,7 +18879,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D33" s="0">
         <v>1</v>
@@ -19076,7 +18971,7 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D37" s="0">
         <v>1</v>
@@ -19145,7 +19040,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D40" s="0">
         <v>1</v>
@@ -19237,7 +19132,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D44" s="0">
         <v>1</v>
@@ -19306,7 +19201,7 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D47" s="0">
         <v>1</v>
@@ -20203,19 +20098,19 @@
         <v>324</v>
       </c>
       <c r="C86" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D86" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F86" t="s">
-        <v>393</v>
+        <v>148</v>
       </c>
       <c r="G86" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
     </row>
     <row r="87">
@@ -20226,19 +20121,19 @@
         <v>325</v>
       </c>
       <c r="C87" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D87" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F87" t="s">
-        <v>394</v>
+        <v>148</v>
       </c>
       <c r="G87" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
     </row>
     <row r="88">
@@ -20249,19 +20144,19 @@
         <v>84</v>
       </c>
       <c r="C88" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D88" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F88" t="s">
-        <v>395</v>
+        <v>148</v>
       </c>
       <c r="G88" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
     </row>
     <row r="89">
@@ -20272,19 +20167,19 @@
         <v>85</v>
       </c>
       <c r="C89" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D89" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F89" t="s">
-        <v>396</v>
+        <v>148</v>
       </c>
       <c r="G89" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
     </row>
     <row r="90">
@@ -20295,19 +20190,19 @@
         <v>86</v>
       </c>
       <c r="C90" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D90" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F90" t="s">
-        <v>397</v>
+        <v>148</v>
       </c>
       <c r="G90" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
     </row>
     <row r="91">
@@ -20318,19 +20213,19 @@
         <v>87</v>
       </c>
       <c r="C91" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D91" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F91" t="s">
-        <v>398</v>
+        <v>148</v>
       </c>
       <c r="G91" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
     </row>
     <row r="92">
@@ -20341,19 +20236,19 @@
         <v>88</v>
       </c>
       <c r="C92" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D92" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F92" t="s">
-        <v>399</v>
+        <v>148</v>
       </c>
       <c r="G92" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="93">
@@ -20364,19 +20259,19 @@
         <v>92</v>
       </c>
       <c r="C93" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D93" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F93" t="s">
-        <v>400</v>
+        <v>148</v>
       </c>
       <c r="G93" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
     </row>
     <row r="94">
@@ -20387,19 +20282,19 @@
         <v>269</v>
       </c>
       <c r="C94" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D94" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F94" t="s">
-        <v>401</v>
+        <v>148</v>
       </c>
       <c r="G94" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
     </row>
     <row r="95">
@@ -20410,19 +20305,19 @@
         <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D95" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F95" t="s">
-        <v>402</v>
+        <v>148</v>
       </c>
       <c r="G95" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
     </row>
     <row r="96">
@@ -20433,19 +20328,19 @@
         <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D96" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F96" t="s">
-        <v>403</v>
+        <v>148</v>
       </c>
       <c r="G96" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
     </row>
     <row r="97">
@@ -20456,19 +20351,19 @@
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D97" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F97" t="s">
-        <v>404</v>
+        <v>148</v>
       </c>
       <c r="G97" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
     </row>
     <row r="98">
@@ -20479,19 +20374,19 @@
         <v>326</v>
       </c>
       <c r="C98" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D98" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F98" t="s">
-        <v>405</v>
+        <v>148</v>
       </c>
       <c r="G98" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
     </row>
     <row r="99">
@@ -20502,19 +20397,19 @@
         <v>96</v>
       </c>
       <c r="C99" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D99" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F99" t="s">
-        <v>406</v>
+        <v>148</v>
       </c>
       <c r="G99" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
     </row>
     <row r="100">
@@ -20525,19 +20420,19 @@
         <v>97</v>
       </c>
       <c r="C100" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D100" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F100" t="s">
-        <v>407</v>
+        <v>148</v>
       </c>
       <c r="G100" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
     </row>
     <row r="101">
@@ -20548,19 +20443,19 @@
         <v>327</v>
       </c>
       <c r="C101" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D101" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F101" t="s">
-        <v>408</v>
+        <v>148</v>
       </c>
       <c r="G101" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
     </row>
     <row r="102">
@@ -20571,19 +20466,19 @@
         <v>98</v>
       </c>
       <c r="C102" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D102" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F102" t="s">
-        <v>409</v>
+        <v>148</v>
       </c>
       <c r="G102" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
     </row>
     <row r="103">
@@ -20594,19 +20489,19 @@
         <v>328</v>
       </c>
       <c r="C103" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D103" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F103" t="s">
-        <v>410</v>
+        <v>148</v>
       </c>
       <c r="G103" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
     </row>
     <row r="104">
@@ -21215,7 +21110,7 @@
         <v>127</v>
       </c>
       <c r="C130" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D130" s="0">
         <v>1</v>
@@ -21238,7 +21133,7 @@
         <v>128</v>
       </c>
       <c r="C131" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D131" s="0">
         <v>1</v>
@@ -21261,7 +21156,7 @@
         <v>129</v>
       </c>
       <c r="C132" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D132" s="0">
         <v>1</v>
@@ -21284,7 +21179,7 @@
         <v>130</v>
       </c>
       <c r="C133" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D133" s="0">
         <v>1</v>
@@ -21330,7 +21225,7 @@
         <v>131</v>
       </c>
       <c r="C135" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D135" s="0">
         <v>1</v>
@@ -21353,7 +21248,7 @@
         <v>132</v>
       </c>
       <c r="C136" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D136" s="0">
         <v>1</v>
@@ -21577,7 +21472,7 @@
         <v>143</v>
       </c>
       <c r="F7" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="G7" t="s">
         <v>339</v>
@@ -22025,7 +21920,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="C27" t="s">
         <v>135</v>
@@ -22040,7 +21935,7 @@
         <v>148</v>
       </c>
       <c r="G27" t="s">
-        <v>462</v>
+        <v>430</v>
       </c>
     </row>
     <row r="28">
@@ -22278,7 +22173,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="C38" t="s">
         <v>135</v>
@@ -22293,7 +22188,7 @@
         <v>149</v>
       </c>
       <c r="G38" t="s">
-        <v>463</v>
+        <v>431</v>
       </c>
     </row>
     <row r="39">
@@ -22761,7 +22656,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="C59" t="s">
         <v>135</v>
@@ -22776,7 +22671,7 @@
         <v>148</v>
       </c>
       <c r="G59" t="s">
-        <v>462</v>
+        <v>430</v>
       </c>
     </row>
     <row r="60">
@@ -22876,7 +22771,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="C64" t="s">
         <v>135</v>
@@ -22891,7 +22786,7 @@
         <v>148</v>
       </c>
       <c r="G64" t="s">
-        <v>463</v>
+        <v>431</v>
       </c>
     </row>
     <row r="65">
@@ -23198,7 +23093,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="C78" t="s">
         <v>135</v>
@@ -23213,7 +23108,7 @@
         <v>148</v>
       </c>
       <c r="G78" t="s">
-        <v>464</v>
+        <v>432</v>
       </c>
     </row>
     <row r="79">
@@ -23313,7 +23208,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="C83" t="s">
         <v>135</v>
@@ -23328,7 +23223,7 @@
         <v>148</v>
       </c>
       <c r="G83" t="s">
-        <v>465</v>
+        <v>433</v>
       </c>
     </row>
     <row r="84">
@@ -23431,19 +23326,19 @@
         <v>324</v>
       </c>
       <c r="C88" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D88" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F88" t="s">
-        <v>443</v>
+        <v>148</v>
       </c>
       <c r="G88" t="s">
-        <v>466</v>
+        <v>434</v>
       </c>
     </row>
     <row r="89">
@@ -23454,19 +23349,19 @@
         <v>325</v>
       </c>
       <c r="C89" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D89" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F89" t="s">
-        <v>444</v>
+        <v>148</v>
       </c>
       <c r="G89" t="s">
-        <v>467</v>
+        <v>435</v>
       </c>
     </row>
     <row r="90">
@@ -23477,19 +23372,19 @@
         <v>84</v>
       </c>
       <c r="C90" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D90" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F90" t="s">
-        <v>445</v>
+        <v>148</v>
       </c>
       <c r="G90" t="s">
-        <v>468</v>
+        <v>436</v>
       </c>
     </row>
     <row r="91">
@@ -23500,19 +23395,19 @@
         <v>85</v>
       </c>
       <c r="C91" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D91" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F91" t="s">
-        <v>446</v>
+        <v>148</v>
       </c>
       <c r="G91" t="s">
-        <v>469</v>
+        <v>437</v>
       </c>
     </row>
     <row r="92">
@@ -23523,19 +23418,19 @@
         <v>86</v>
       </c>
       <c r="C92" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D92" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F92" t="s">
-        <v>447</v>
+        <v>148</v>
       </c>
       <c r="G92" t="s">
-        <v>470</v>
+        <v>438</v>
       </c>
     </row>
     <row r="93">
@@ -23546,19 +23441,19 @@
         <v>87</v>
       </c>
       <c r="C93" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D93" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F93" t="s">
-        <v>448</v>
+        <v>148</v>
       </c>
       <c r="G93" t="s">
-        <v>471</v>
+        <v>439</v>
       </c>
     </row>
     <row r="94">
@@ -23569,19 +23464,19 @@
         <v>88</v>
       </c>
       <c r="C94" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D94" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F94" t="s">
-        <v>449</v>
+        <v>148</v>
       </c>
       <c r="G94" t="s">
-        <v>472</v>
+        <v>440</v>
       </c>
     </row>
     <row r="95">
@@ -23592,19 +23487,19 @@
         <v>92</v>
       </c>
       <c r="C95" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D95" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" t="s">
+        <v>428</v>
+      </c>
+      <c r="F95" t="s">
+        <v>148</v>
+      </c>
+      <c r="G95" t="s">
         <v>441</v>
-      </c>
-      <c r="F95" t="s">
-        <v>450</v>
-      </c>
-      <c r="G95" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="96">
@@ -23615,19 +23510,19 @@
         <v>93</v>
       </c>
       <c r="C96" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D96" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F96" t="s">
-        <v>451</v>
+        <v>148</v>
       </c>
       <c r="G96" t="s">
-        <v>474</v>
+        <v>442</v>
       </c>
     </row>
     <row r="97">
@@ -23635,22 +23530,22 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="C97" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D97" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F97" t="s">
-        <v>452</v>
+        <v>148</v>
       </c>
       <c r="G97" t="s">
-        <v>475</v>
+        <v>443</v>
       </c>
     </row>
     <row r="98">
@@ -23661,19 +23556,19 @@
         <v>94</v>
       </c>
       <c r="C98" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D98" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F98" t="s">
-        <v>453</v>
+        <v>148</v>
       </c>
       <c r="G98" t="s">
-        <v>474</v>
+        <v>442</v>
       </c>
     </row>
     <row r="99">
@@ -23684,19 +23579,19 @@
         <v>95</v>
       </c>
       <c r="C99" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D99" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F99" t="s">
-        <v>454</v>
+        <v>148</v>
       </c>
       <c r="G99" t="s">
-        <v>474</v>
+        <v>442</v>
       </c>
     </row>
     <row r="100">
@@ -23707,19 +23602,19 @@
         <v>326</v>
       </c>
       <c r="C100" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D100" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F100" t="s">
-        <v>455</v>
+        <v>148</v>
       </c>
       <c r="G100" t="s">
-        <v>476</v>
+        <v>444</v>
       </c>
     </row>
     <row r="101">
@@ -23730,19 +23625,19 @@
         <v>96</v>
       </c>
       <c r="C101" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D101" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F101" t="s">
-        <v>456</v>
+        <v>148</v>
       </c>
       <c r="G101" t="s">
-        <v>474</v>
+        <v>442</v>
       </c>
     </row>
     <row r="102">
@@ -23750,22 +23645,22 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="C102" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D102" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F102" t="s">
-        <v>457</v>
+        <v>148</v>
       </c>
       <c r="G102" t="s">
-        <v>477</v>
+        <v>445</v>
       </c>
     </row>
     <row r="103">
@@ -23776,19 +23671,19 @@
         <v>97</v>
       </c>
       <c r="C103" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D103" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F103" t="s">
-        <v>458</v>
+        <v>148</v>
       </c>
       <c r="G103" t="s">
-        <v>474</v>
+        <v>442</v>
       </c>
     </row>
     <row r="104">
@@ -23799,19 +23694,19 @@
         <v>327</v>
       </c>
       <c r="C104" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D104" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F104" t="s">
-        <v>459</v>
+        <v>148</v>
       </c>
       <c r="G104" t="s">
-        <v>478</v>
+        <v>446</v>
       </c>
     </row>
     <row r="105">
@@ -23822,19 +23717,19 @@
         <v>98</v>
       </c>
       <c r="C105" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D105" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F105" t="s">
-        <v>460</v>
+        <v>148</v>
       </c>
       <c r="G105" t="s">
-        <v>474</v>
+        <v>442</v>
       </c>
     </row>
     <row r="106">
@@ -23845,19 +23740,19 @@
         <v>328</v>
       </c>
       <c r="C106" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D106" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="F106" t="s">
-        <v>461</v>
+        <v>148</v>
       </c>
       <c r="G106" t="s">
-        <v>479</v>
+        <v>447</v>
       </c>
     </row>
     <row r="107">
@@ -24072,7 +23967,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="C116" t="s">
         <v>135</v>
@@ -24087,7 +23982,7 @@
         <v>148</v>
       </c>
       <c r="G116" t="s">
-        <v>480</v>
+        <v>448</v>
       </c>
     </row>
     <row r="117">
@@ -24187,7 +24082,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="C121" t="s">
         <v>135</v>
@@ -24202,7 +24097,7 @@
         <v>148</v>
       </c>
       <c r="G121" t="s">
-        <v>481</v>
+        <v>449</v>
       </c>
     </row>
     <row r="122">
@@ -24532,7 +24427,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="C136" t="s">
         <v>138</v>
@@ -24544,10 +24439,10 @@
         <v>371</v>
       </c>
       <c r="F136" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="G136" t="s">
-        <v>482</v>
+        <v>450</v>
       </c>
     </row>
     <row r="137">
@@ -24647,7 +24542,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="C141" t="s">
         <v>138</v>
@@ -24659,10 +24554,10 @@
         <v>371</v>
       </c>
       <c r="F141" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="G141" t="s">
-        <v>483</v>
+        <v>451</v>
       </c>
     </row>
     <row r="142">

</xml_diff>